<commit_message>
thời khóa biểu nâng cao
</commit_message>
<xml_diff>
--- a/cách sử dụng git/Tóm tắt lý thuyết.xlsx
+++ b/cách sử dụng git/Tóm tắt lý thuyết.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAPTOP\Desktop\Hanh_code\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD0BEC7-9B4E-4146-B391-A856C4C00474}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{581A51B4-FC8D-4CE3-BB41-899C4C2C09B5}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Lý thuyết" sheetId="1" r:id="rId1"/>
     <sheet name="Bài tập" sheetId="2" r:id="rId2"/>
+    <sheet name="QA" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>Thẻ input</t>
   </si>
@@ -1659,17 +1654,74 @@
       </rPr>
       <t>&gt;</t>
     </r>
+  </si>
+  <si>
+    <t>&lt;table&gt;</t>
+  </si>
+  <si>
+    <t>&lt;thead&gt;</t>
+  </si>
+  <si>
+    <t>&lt;tr&gt;</t>
+  </si>
+  <si>
+    <t>&lt;th&gt;thead01&lt;/th&gt;</t>
+  </si>
+  <si>
+    <t>&lt;th&gt;thead02&lt;/th&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/tr&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/thead&gt;</t>
+  </si>
+  <si>
+    <t>&lt;tfoot&gt;</t>
+  </si>
+  <si>
+    <t>&lt;td&gt;tfoot01&lt;/td&gt;</t>
+  </si>
+  <si>
+    <t>&lt;td&gt;tfoot02&lt;/td&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/tfoot&gt;</t>
+  </si>
+  <si>
+    <t>&lt;tbody&gt;</t>
+  </si>
+  <si>
+    <t>&lt;td&gt;tbody01&lt;/td&gt;</t>
+  </si>
+  <si>
+    <t>&lt;td&gt;tbody02&lt;/td&gt;</t>
+  </si>
+  <si>
+    <t>&lt;td&gt;tbody03&lt;/td&gt;</t>
+  </si>
+  <si>
+    <t>&lt;td&gt;tbody04&lt;/td&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/tbody&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/table&gt;</t>
+  </si>
+  <si>
+    <t>Heading</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -1698,6 +1750,14 @@
       <name val="Lucida Console"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1707,9 +1767,18 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -1719,11 +1788,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1752,16 +1824,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>617562</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>53190</xdr:rowOff>
+      <xdr:colOff>608037</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>162047</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EF569F6-9000-460C-9AA5-DB93F2B73AE7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6EF569F6-9000-460C-9AA5-DB93F2B73AE7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1797,15 +1869,15 @@
     <xdr:to>
       <xdr:col>36</xdr:col>
       <xdr:colOff>280069</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>149913</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>68270</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37806DB5-0A91-4108-BCE6-3719C4A39C10}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{37806DB5-0A91-4108-BCE6-3719C4A39C10}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1841,15 +1913,15 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>376457</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>161171</xdr:rowOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>79528</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C1253D6-9534-43AF-9B36-E199F44DB24B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8C1253D6-9534-43AF-9B36-E199F44DB24B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1885,15 +1957,15 @@
     <xdr:to>
       <xdr:col>36</xdr:col>
       <xdr:colOff>420819</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>84981</xdr:rowOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>3338</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23D1A57B-A1C9-4F72-AA45-0721B58625DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{23D1A57B-A1C9-4F72-AA45-0721B58625DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1937,7 +2009,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6592CF3C-755A-4984-AD6A-26E99B659410}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6592CF3C-755A-4984-AD6A-26E99B659410}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1981,7 +2053,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67F58117-8EF4-4CDD-9F34-0E89C9D97015}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{67F58117-8EF4-4CDD-9F34-0E89C9D97015}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2016,7 +2088,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>646286</xdr:colOff>
+      <xdr:colOff>608186</xdr:colOff>
       <xdr:row>142</xdr:row>
       <xdr:rowOff>116696</xdr:rowOff>
     </xdr:to>
@@ -2025,7 +2097,7 @@
         <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96F94067-969B-48BB-BA2D-CA80D285A7B0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{96F94067-969B-48BB-BA2D-CA80D285A7B0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2069,7 +2141,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC810811-BE7B-4B97-9994-27EF8BB7576E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AC810811-BE7B-4B97-9994-27EF8BB7576E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2113,7 +2185,7 @@
         <xdr:cNvPr id="10" name="Picture 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E192DB8C-8084-483C-89BC-33A19EE2243C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E192DB8C-8084-483C-89BC-33A19EE2243C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2157,7 +2229,7 @@
         <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4239A290-42CD-4760-801B-F87FF3EBBD9E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4239A290-42CD-4760-801B-F87FF3EBBD9E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2201,7 +2273,7 @@
         <xdr:cNvPr id="12" name="Picture 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECBC413C-C95B-4FED-8631-91E73467FC37}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ECBC413C-C95B-4FED-8631-91E73467FC37}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2245,7 +2317,7 @@
         <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F24226A-454A-46EC-978F-624816C19D25}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7F24226A-454A-46EC-978F-624816C19D25}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2289,7 +2361,7 @@
         <xdr:cNvPr id="14" name="Picture 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3F53535-9B33-496B-91F8-90624DC9C2CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B3F53535-9B33-496B-91F8-90624DC9C2CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2333,7 +2405,7 @@
         <xdr:cNvPr id="15" name="Picture 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B395BD5-DF7C-49B1-9091-3555E546ED03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B395BD5-DF7C-49B1-9091-3555E546ED03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2377,7 +2449,7 @@
         <xdr:cNvPr id="16" name="Picture 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF08EA8B-BF5A-4D46-9F15-7CB1E0464502}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF08EA8B-BF5A-4D46-9F15-7CB1E0464502}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2421,7 +2493,7 @@
         <xdr:cNvPr id="17" name="Picture 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23C32360-F3EE-4E58-9281-7941D9E48700}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{23C32360-F3EE-4E58-9281-7941D9E48700}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2456,7 +2528,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>615299</xdr:colOff>
+      <xdr:colOff>605774</xdr:colOff>
       <xdr:row>330</xdr:row>
       <xdr:rowOff>160433</xdr:rowOff>
     </xdr:to>
@@ -2465,7 +2537,7 @@
         <xdr:cNvPr id="18" name="Picture 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAA5B843-B57C-4DE5-B111-1BFE059502C8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DAA5B843-B57C-4DE5-B111-1BFE059502C8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2509,7 +2581,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48C25F48-0D7F-4466-AAA9-29A0087B5E08}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{48C25F48-0D7F-4466-AAA9-29A0087B5E08}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2580,7 +2652,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50EB1272-529B-4BFE-8D06-0A5D4FAE7E47}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{50EB1272-529B-4BFE-8D06-0A5D4FAE7E47}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2624,7 +2696,7 @@
         <xdr:cNvPr id="21" name="Picture 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F40B230-60A3-4A8B-A6A2-2DDCD9BB2454}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3F40B230-60A3-4A8B-A6A2-2DDCD9BB2454}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2642,6 +2714,196 @@
         <a:xfrm>
           <a:off x="6580909" y="62253091"/>
           <a:ext cx="3552381" cy="3238095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>66357</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>161643</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26003250" y="20764500"/>
+          <a:ext cx="2542857" cy="2257143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>197809</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>77262</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="27649714" y="5197929"/>
+          <a:ext cx="6838095" cy="2390476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>100298</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>104167</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23880536" y="5225143"/>
+          <a:ext cx="3161905" cy="4866667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>598713</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>190916</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>32047</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23254606" y="11702143"/>
+          <a:ext cx="7552381" cy="4876190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>80714</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>27952</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="31840714" y="11974286"/>
+          <a:ext cx="7428571" cy="4980952"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2673,7 +2935,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC661A39-5B67-42DE-A646-067F7F2B016A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AC661A39-5B67-42DE-A646-067F7F2B016A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2697,6 +2959,170 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>113371</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>75667</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="7428571" cy="4266667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="152400" y="1400175"/>
+          <a:ext cx="7048500" cy="1019175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rounded Rectangular Callout 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7248525" y="266700"/>
+          <a:ext cx="2990850" cy="1038225"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -50769"/>
+            <a:gd name="adj2" fmla="val 89105"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Phần</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> này dung cách nào? table hay thẻ &lt;p align ="center"&gt;</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2991,33 +3417,161 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C33C9587-ECE4-4964-B103-2AD1719CA9A0}">
-  <dimension ref="A225:J360"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AN360"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AH304" sqref="AH304"/>
+    <sheetView topLeftCell="AG61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BA61" sqref="BA61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="39" max="39" width="9.140625" style="2"/>
+  </cols>
   <sheetData>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="40:40" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="AN1" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="58" spans="39:39" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="AM58" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:10" ht="20" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="J226" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="227" spans="1:10" ht="20" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>1</v>
       </c>
@@ -3025,12 +3579,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="228" spans="1:10" ht="20" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="J228" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="229" spans="1:10" ht="20" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>2</v>
       </c>
@@ -3038,12 +3592,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="230" spans="1:10" ht="20" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="J230" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="231" spans="1:10" ht="20" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>3</v>
       </c>
@@ -3051,12 +3605,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="232" spans="1:10" ht="20" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="J232" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="233" spans="1:10" ht="20" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>4</v>
       </c>
@@ -3064,113 +3618,112 @@
         <v>19</v>
       </c>
     </row>
-    <row r="234" spans="1:10" ht="20" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
       <c r="J234" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="331" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="337" spans="1:1" ht="20" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:1" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="338" spans="1:1" ht="20" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:1" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="339" spans="1:1" ht="20" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:1" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="340" spans="1:1" ht="20" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:1" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="341" spans="1:1" ht="20" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:1" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="342" spans="1:1" ht="20" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:1" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="343" spans="1:1" ht="20" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:1" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="354" spans="1:1" ht="20" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:1" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="355" spans="1:1" ht="20" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:1" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="356" spans="1:1" ht="20" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:1" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="357" spans="1:1" ht="20" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:1" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="358" spans="1:1" ht="20" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:1" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="359" spans="1:1" ht="20" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:1" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="360" spans="1:1" ht="20" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:1" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
         <v>27</v>
       </c>
@@ -3183,14 +3736,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5851C8C-A508-40CF-A219-C84856BA7022}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
điểm trung bình toán lý hóa
</commit_message>
<xml_diff>
--- a/cách sử dụng git/Tóm tắt lý thuyết.xlsx
+++ b/cách sử dụng git/Tóm tắt lý thuyết.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Lý thuyết" sheetId="1" r:id="rId1"/>
     <sheet name="Bài tập" sheetId="2" r:id="rId2"/>
     <sheet name="QA" sheetId="3" r:id="rId3"/>
+    <sheet name="Biến, toán tử" sheetId="4" r:id="rId4"/>
+    <sheet name="Bài tập 1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -1833,7 +1835,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6EF569F6-9000-460C-9AA5-DB93F2B73AE7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EF569F6-9000-460C-9AA5-DB93F2B73AE7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1877,7 +1879,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{37806DB5-0A91-4108-BCE6-3719C4A39C10}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37806DB5-0A91-4108-BCE6-3719C4A39C10}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1921,7 +1923,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8C1253D6-9534-43AF-9B36-E199F44DB24B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C1253D6-9534-43AF-9B36-E199F44DB24B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1965,7 +1967,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{23D1A57B-A1C9-4F72-AA45-0721B58625DC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23D1A57B-A1C9-4F72-AA45-0721B58625DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2009,7 +2011,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6592CF3C-755A-4984-AD6A-26E99B659410}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6592CF3C-755A-4984-AD6A-26E99B659410}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2053,7 +2055,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{67F58117-8EF4-4CDD-9F34-0E89C9D97015}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67F58117-8EF4-4CDD-9F34-0E89C9D97015}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2097,7 +2099,7 @@
         <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{96F94067-969B-48BB-BA2D-CA80D285A7B0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96F94067-969B-48BB-BA2D-CA80D285A7B0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2141,7 +2143,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AC810811-BE7B-4B97-9994-27EF8BB7576E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC810811-BE7B-4B97-9994-27EF8BB7576E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2185,7 +2187,7 @@
         <xdr:cNvPr id="10" name="Picture 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E192DB8C-8084-483C-89BC-33A19EE2243C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E192DB8C-8084-483C-89BC-33A19EE2243C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2229,7 +2231,7 @@
         <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4239A290-42CD-4760-801B-F87FF3EBBD9E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4239A290-42CD-4760-801B-F87FF3EBBD9E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2273,7 +2275,7 @@
         <xdr:cNvPr id="12" name="Picture 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ECBC413C-C95B-4FED-8631-91E73467FC37}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECBC413C-C95B-4FED-8631-91E73467FC37}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2317,7 +2319,7 @@
         <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7F24226A-454A-46EC-978F-624816C19D25}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F24226A-454A-46EC-978F-624816C19D25}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2361,7 +2363,7 @@
         <xdr:cNvPr id="14" name="Picture 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B3F53535-9B33-496B-91F8-90624DC9C2CE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3F53535-9B33-496B-91F8-90624DC9C2CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2405,7 +2407,7 @@
         <xdr:cNvPr id="15" name="Picture 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B395BD5-DF7C-49B1-9091-3555E546ED03}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B395BD5-DF7C-49B1-9091-3555E546ED03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2449,7 +2451,7 @@
         <xdr:cNvPr id="16" name="Picture 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF08EA8B-BF5A-4D46-9F15-7CB1E0464502}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF08EA8B-BF5A-4D46-9F15-7CB1E0464502}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2493,7 +2495,7 @@
         <xdr:cNvPr id="17" name="Picture 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{23C32360-F3EE-4E58-9281-7941D9E48700}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23C32360-F3EE-4E58-9281-7941D9E48700}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2537,7 +2539,7 @@
         <xdr:cNvPr id="18" name="Picture 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DAA5B843-B57C-4DE5-B111-1BFE059502C8}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAA5B843-B57C-4DE5-B111-1BFE059502C8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2581,7 +2583,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{48C25F48-0D7F-4466-AAA9-29A0087B5E08}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48C25F48-0D7F-4466-AAA9-29A0087B5E08}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2652,7 +2654,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{50EB1272-529B-4BFE-8D06-0A5D4FAE7E47}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50EB1272-529B-4BFE-8D06-0A5D4FAE7E47}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2696,7 +2698,7 @@
         <xdr:cNvPr id="21" name="Picture 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3F40B230-60A3-4A8B-A6A2-2DDCD9BB2454}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F40B230-60A3-4A8B-A6A2-2DDCD9BB2454}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2935,7 +2937,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AC661A39-5B67-42DE-A646-067F7F2B016A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC661A39-5B67-42DE-A646-067F7F2B016A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3123,6 +3125,384 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>142019</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>104143</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4953000"/>
+          <a:ext cx="6847619" cy="5057143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rounded Rectangular Callout 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6391275" y="6019800"/>
+          <a:ext cx="2990850" cy="1038225"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -50769"/>
+            <a:gd name="adj2" fmla="val 89105"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Cách</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> tạo chữ nhỏ ở dưới  có phải là dùng size để biến hóa không?</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>265905</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85357</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6361905" cy="2942857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>94324</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>94786</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705600" y="190500"/>
+          <a:ext cx="7409524" cy="3714286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>332419</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>75643</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3048000"/>
+          <a:ext cx="7647619" cy="4457143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>237105</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>94738</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="7810500"/>
+          <a:ext cx="8161905" cy="4095238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>256228</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>28000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8534400" y="8001000"/>
+          <a:ext cx="7571428" cy="4600000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>422440</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>28071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="612321" y="12573000"/>
+          <a:ext cx="5933333" cy="4028571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>522971</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>56643</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="7228571" cy="4057143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3417,7 +3797,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3754,8 +4134,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="B70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>